<commit_message>
add write start and end
</commit_message>
<xml_diff>
--- a/public/files/tcherenkovskiy/report.xlsx
+++ b/public/files/tcherenkovskiy/report.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="35">
   <si>
     <t>Расход электроэнергии за</t>
   </si>
@@ -67,13 +67,34 @@
     <t>конец</t>
   </si>
   <si>
+    <t>2283Г</t>
+  </si>
+  <si>
     <t>ПЗР к бурению</t>
   </si>
   <si>
     <t>бурение</t>
   </si>
   <si>
+    <t>2022-01-26 20:00</t>
+  </si>
+  <si>
+    <t>2022-02-01 20:44</t>
+  </si>
+  <si>
     <t>Итого по скважине</t>
+  </si>
+  <si>
+    <t>666Г</t>
+  </si>
+  <si>
+    <t>2022-02-01 20:45</t>
+  </si>
+  <si>
+    <t>2022-02-02 20:45</t>
+  </si>
+  <si>
+    <t>2022-02-28 20:45</t>
   </si>
   <si>
     <t>переход</t>
@@ -1141,9 +1162,11 @@
       <c r="AL9" s="20"/>
     </row>
     <row r="10" ht="13.8" customHeight="1" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A10" s="21"/>
+      <c r="A10" s="21" t="s">
+        <v>16</v>
+      </c>
       <c r="B10" s="22" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C10" s="23"/>
       <c r="D10" s="24"/>
@@ -1191,13 +1214,13 @@
     <row r="11" ht="13.8" customHeight="1" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A11" s="21"/>
       <c r="B11" s="32" t="s">
-        <v>17</v>
-      </c>
-      <c r="C11" s="33">
-        <v>44527.08333333333</v>
-      </c>
-      <c r="D11" s="34">
-        <v>44538.25</v>
+        <v>18</v>
+      </c>
+      <c r="C11" s="33" t="s">
+        <v>19</v>
+      </c>
+      <c r="D11" s="34" t="s">
+        <v>20</v>
       </c>
       <c r="E11" s="35"/>
       <c r="F11" s="35"/>
@@ -1243,7 +1266,7 @@
     <row r="12" ht="15.75" customHeight="1" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A12" s="21"/>
       <c r="B12" s="38" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="C12" s="38"/>
       <c r="D12" s="38"/>
@@ -1382,15 +1405,17 @@
       <c r="AL12" s="20"/>
     </row>
     <row r="13" ht="13.8" customHeight="1" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A13" s="21"/>
+      <c r="A13" s="21" t="s">
+        <v>22</v>
+      </c>
       <c r="B13" s="22" t="s">
-        <v>16</v>
-      </c>
-      <c r="C13" s="23">
-        <v>44538.25</v>
-      </c>
-      <c r="D13" s="24">
-        <v>44539.04166666667</v>
+        <v>17</v>
+      </c>
+      <c r="C13" s="23" t="s">
+        <v>23</v>
+      </c>
+      <c r="D13" s="24" t="s">
+        <v>24</v>
       </c>
       <c r="E13" s="25"/>
       <c r="F13" s="25"/>
@@ -1436,13 +1461,13 @@
     <row r="14" ht="13.8" customHeight="1" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A14" s="21"/>
       <c r="B14" s="32" t="s">
-        <v>17</v>
-      </c>
-      <c r="C14" s="33">
-        <v>44539.04166666667</v>
-      </c>
-      <c r="D14" s="33">
-        <v>44547.41666666667</v>
+        <v>18</v>
+      </c>
+      <c r="C14" s="33" t="s">
+        <v>24</v>
+      </c>
+      <c r="D14" s="33" t="s">
+        <v>25</v>
       </c>
       <c r="E14" s="43"/>
       <c r="F14" s="43"/>
@@ -1488,7 +1513,7 @@
     <row r="15" ht="15.75" customHeight="1" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A15" s="21"/>
       <c r="B15" s="38" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="C15" s="38"/>
       <c r="D15" s="38"/>
@@ -1629,7 +1654,7 @@
     <row r="16" ht="13.8" customHeight="1" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A16" s="21"/>
       <c r="B16" s="22" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C16" s="23">
         <v>44547.41666666667</v>
@@ -1681,7 +1706,7 @@
     <row r="17" ht="13.8" customHeight="1" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A17" s="21"/>
       <c r="B17" s="32" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C17" s="33">
         <v>44548.25</v>
@@ -1733,7 +1758,7 @@
     <row r="18" ht="15.75" customHeight="1" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A18" s="21"/>
       <c r="B18" s="38" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="C18" s="38"/>
       <c r="D18" s="38"/>
@@ -1874,7 +1899,7 @@
     <row r="19" ht="13.8" customHeight="1" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A19" s="21"/>
       <c r="B19" s="22" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C19" s="50">
         <v>44558.33333333333</v>
@@ -1926,13 +1951,13 @@
     <row r="20" ht="13.8" customHeight="1" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A20" s="21"/>
       <c r="B20" s="32" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C20" s="33">
         <v>44559</v>
       </c>
       <c r="D20" s="49" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="E20" s="43"/>
       <c r="F20" s="43"/>
@@ -1978,7 +2003,7 @@
     <row r="21" ht="15.75" customHeight="1" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A21" s="21"/>
       <c r="B21" s="38" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="C21" s="38"/>
       <c r="D21" s="38"/>
@@ -2151,7 +2176,7 @@
       <c r="AF22" s="55"/>
       <c r="AG22" s="55"/>
       <c r="AH22" s="55" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="AI22" s="55"/>
       <c r="AJ22" s="56">
@@ -2308,7 +2333,7 @@
     <row r="28" ht="13.8" customHeight="1" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A28" s="11"/>
       <c r="B28" s="3" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="C28" s="3"/>
       <c r="D28" s="3"/>
@@ -2430,7 +2455,7 @@
     <row r="31" ht="13.8" customHeight="1" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A31" s="64"/>
       <c r="B31" s="3" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="C31" s="3"/>
       <c r="D31" s="3"/>
@@ -2482,7 +2507,7 @@
       <c r="J32" s="62"/>
       <c r="K32" s="61"/>
       <c r="L32" s="67" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="M32" s="67"/>
       <c r="N32" s="67"/>
@@ -2554,7 +2579,7 @@
     <row r="34" ht="13.8" customHeight="1" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A34" s="64"/>
       <c r="B34" s="3" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="C34" s="3"/>
       <c r="D34" s="3"/>
@@ -2606,7 +2631,7 @@
       <c r="J35" s="61"/>
       <c r="K35" s="61"/>
       <c r="L35" s="67" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="M35" s="67"/>
       <c r="N35" s="67"/>
@@ -2678,7 +2703,7 @@
     <row r="37" ht="13.8" customHeight="1" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A37" s="64"/>
       <c r="B37" s="3" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="C37" s="3"/>
       <c r="D37" s="61"/>
@@ -2720,7 +2745,7 @@
     <row r="38" ht="13.8" customHeight="1" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A38" s="64"/>
       <c r="B38" s="3" t="s">
-        <v>26</v>
+        <v>33</v>
       </c>
       <c r="C38" s="3"/>
       <c r="D38" s="61"/>
@@ -2802,7 +2827,7 @@
     <row r="40" ht="13.8" customHeight="1" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A40" s="64"/>
       <c r="B40" s="3" t="s">
-        <v>27</v>
+        <v>34</v>
       </c>
       <c r="C40" s="3"/>
       <c r="D40" s="3"/>

</xml_diff>